<commit_message>
popup delete and import data excel fix
</commit_message>
<xml_diff>
--- a/public/Datausers/data-user.xlsx
+++ b/public/Datausers/data-user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A9EF0-5C50-4275-BDF1-C84CCEC9CEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A4099C-A49E-4009-AE48-572CC316B0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,13 +37,13 @@
     <t>dading1</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>imam</t>
   </si>
   <si>
-    <t>name</t>
+    <t>users</t>
+  </si>
+  <si>
+    <t>nama</t>
   </si>
 </sst>
 </file>
@@ -931,9 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -969,21 +967,21 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>

</xml_diff>